<commit_message>
Planing of the next Meeting
</commit_message>
<xml_diff>
--- a/HelepMe/ManagementSet/Planing/toDolist.xlsx
+++ b/HelepMe/ManagementSet/Planing/toDolist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>editeur</t>
   </si>
@@ -40,6 +40,24 @@
   </si>
   <si>
     <t>Project</t>
+  </si>
+  <si>
+    <t>Clovis</t>
+  </si>
+  <si>
+    <t>helpMe</t>
+  </si>
+  <si>
+    <t>Quickoff</t>
+  </si>
+  <si>
+    <t>Intro et Spec</t>
+  </si>
+  <si>
+    <t>Gilles</t>
+  </si>
+  <si>
+    <t>Design</t>
   </si>
 </sst>
 </file>
@@ -55,12 +73,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,8 +99,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -395,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,6 +459,62 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>42975</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42975</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1">
+        <v>42982</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42975</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42982</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>